<commit_message>
* testing xlsx with different params
</commit_message>
<xml_diff>
--- a/Nodejs/XLSXTest/GearConfig.xlsx
+++ b/Nodejs/XLSXTest/GearConfig.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lzg/Workspace/GitHub/Exercise/Nodejs/XLSXTest/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Gear" sheetId="1" r:id="rId1"/>
+    <sheet name="ShadowGear-1" sheetId="2" r:id="rId2"/>
+    <sheet name="ShadowGear-2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <t>GearID</t>
   </si>
@@ -179,10 +189,15 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -510,19 +525,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.83203125" customWidth="1"/>
     <col min="14" max="14" width="18.1640625" customWidth="1"/>
     <col min="15" max="15" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +596,7 @@
       <c r="V1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -608,7 +633,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -637,26 +662,307 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="X1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4">
+        <v>100001</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3">
+        <v>500</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4">
+        <v>100002</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3">
+        <v>400</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="X1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4">
+        <v>200001</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3">
+        <v>500</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4">
+        <v>200002</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3">
+        <v>40</v>
+      </c>
+      <c r="F3" s="3">
+        <v>400</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>